<commit_message>
loading in dataframes / preparation for comment collection
</commit_message>
<xml_diff>
--- a/data/df_videos_2021.xlsx
+++ b/data/df_videos_2021.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzobehna/projects/Social-Computing_Final-Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1C54D5-376B-9C47-BEB6-F634D3F8B252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8931ECA0-A8A8-C142-BF65-FD01080C3C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{F49F7BFC-9310-4561-B399-0EB798D3E0F1}"/>
+    <workbookView xWindow="15140" yWindow="760" windowWidth="15100" windowHeight="18880" xr2:uid="{F49F7BFC-9310-4561-B399-0EB798D3E0F1}"/>
   </bookViews>
   <sheets>
     <sheet name="df_videos_2021" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">df_videos_2021!$A$1:$J$21</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">df_videos_2021!$A$1:$J$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="143">
   <si>
     <t>video_id</t>
   </si>
@@ -852,6 +852,38 @@
   <si>
     <t>video off topic / song about AI</t>
   </si>
+  <si>
+    <t>5q87K1WaoFI</t>
+  </si>
+  <si>
+    <t>Computer Scientist Explains Machine Learning in 5 Levels of Difficulty | WIRED</t>
+  </si>
+  <si>
+    <t>WIRED</t>
+  </si>
+  <si>
+    <t>UCftwRNsjfRo08xYE31tkiyw</t>
+  </si>
+  <si>
+    <t>2021-08-18T16:00:08Z</t>
+  </si>
+  <si>
+    <t>WIRED has challenged computer scientist and Hidden Door cofounder and CEO Hilary Mason to explain machine learning to 5 different people; a child, teen, a college student, a grad student and an expert.
+Still haven‚Äôt subscribed to WIRED on YouTube? ‚ñ∫‚ñ∫ http://wrd.cm/15fP7B7 _x000D_
+Listen to the Get WIRED podcast  ‚ñ∫‚ñ∫ https://link.chtbl.com/wired-ytc-desc_x000D_
+Want more WIRED? Get the magazine ‚ñ∫‚ñ∫ https://subscribe.wired.com/subscribe/splits/wired/WIR_YouTube?source=EDT_WIR_YouTube_0_Video_Description_ZZ_x000D_
+_x000D_
+Get more incredible stories on science and tech with our daily newsletter: https://wrd.cm/DailyYT_x000D_
+_x000D_
+Also, check out the free WIRED channel on Roku, Apple TV, Amazon Fire TV, and Android TV. Here you can find your favorite WIRED shows and new episodes of our latest hit series Tradecraft._x000D_
+_x000D_
+ABOUT WIRED_x000D_
+WIRED is where tomorrow is realized. Through thought-provoking stories and videos, WIRED explores the future of business, innovation, and culture.
+Computer Scientist Explains Machine Learning in 5 Levels of Difficulty | WIRED</t>
+  </si>
+  <si>
+    <t>['5 levels', '5 levels machine learning', '5 levels of machine learning', 'computer science', 'computer scientist', 'explanation machine learning', 'hidden door', 'innovation', 'machine learned', 'machine learning computer scientist', 'machine learning explained', 'machine learning explanation', 'machine learning hidden door', 'machine learning wired', 'machine learning youtube', 'ott 5 levels', 'science &amp; tech', 'science &amp; technology', 'wired', 'wired 5 levels', 'wired computer science', 'wired machine learning']</t>
+  </si>
 </sst>
 </file>
 
@@ -898,13 +930,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,8 +998,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F98F141-3692-4D16-945E-CD8DFCE722B0}" name="df_videos_2021" displayName="df_videos_2021" ref="A1:K21" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:K21" xr:uid="{4F98F141-3692-4D16-945E-CD8DFCE722B0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F98F141-3692-4D16-945E-CD8DFCE722B0}" name="df_videos_2021" displayName="df_videos_2021" ref="A1:K22" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:K22" xr:uid="{4F98F141-3692-4D16-945E-CD8DFCE722B0}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{005DA329-7D7D-4AD1-92A1-E464377DF4BB}" uniqueName="1" name="video_id" queryTableFieldId="1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{87C0455B-0430-4FD0-BAEB-9A94539AB557}" uniqueName="2" name="video_title" queryTableFieldId="2" dataDxfId="5"/>
@@ -1301,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3348C916-9FDD-4743-99E3-819D100737FB}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1385,374 +1418,371 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1">
-        <v>44548.666701388887</v>
-      </c>
-      <c r="F3">
-        <v>2592146</v>
-      </c>
-      <c r="G3">
-        <v>6970</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3">
-        <v>27</v>
+    <row r="3" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="6">
+        <v>2314382</v>
+      </c>
+      <c r="G3" s="6">
+        <v>2170</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J3" s="6">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3">
-        <v>44461.739212962966</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2553357</v>
-      </c>
-      <c r="G4" s="2">
-        <v>8605</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44548.666701388887</v>
+      </c>
+      <c r="F4">
+        <v>2592146</v>
+      </c>
+      <c r="G4">
+        <v>6970</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4">
         <v>27</v>
-      </c>
-      <c r="J4" s="2">
-        <v>28</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E5" s="3">
-        <v>44272.915462962963</v>
+        <v>44461.739212962966</v>
       </c>
       <c r="F5" s="2">
-        <v>2182846</v>
+        <v>2553357</v>
       </c>
       <c r="G5" s="2">
-        <v>523</v>
+        <v>8605</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="J5" s="2">
         <v>28</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E6" s="3">
-        <v>44413.983935185184</v>
+        <v>44272.915462962963</v>
       </c>
       <c r="F6" s="2">
-        <v>2108952</v>
+        <v>2182846</v>
       </c>
       <c r="G6" s="2">
-        <v>3317</v>
+        <v>523</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="J6" s="2">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="1">
-        <v>44227.750127314815</v>
-      </c>
-      <c r="F7">
-        <v>1875122</v>
-      </c>
-      <c r="G7">
-        <v>2705</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7">
-        <v>24</v>
+      <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44413.983935185184</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2108952</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3317</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="2">
+        <v>23</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E8" s="1">
-        <v>44216.500011574077</v>
+        <v>44227.750127314815</v>
       </c>
       <c r="F8">
-        <v>1132089</v>
+        <v>1875122</v>
       </c>
       <c r="G8">
-        <v>1380</v>
+        <v>2705</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J8">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="3">
-        <v>44197.833449074074</v>
-      </c>
-      <c r="F9" s="2">
-        <v>991863</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1000</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="2">
-        <v>27</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>131</v>
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44216.500011574077</v>
+      </c>
+      <c r="F9">
+        <v>1132089</v>
+      </c>
+      <c r="G9">
+        <v>1380</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E10" s="3">
-        <v>44304.8283912037</v>
+        <v>44197.833449074074</v>
       </c>
       <c r="F10" s="2">
-        <v>855994</v>
+        <v>991863</v>
       </c>
       <c r="G10" s="2">
-        <v>1922</v>
+        <v>1000</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J10" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="5">
-        <v>44266.709444444445</v>
-      </c>
-      <c r="F11" s="4">
-        <v>652159</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1235</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J11" s="4">
-        <v>27</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>133</v>
+      <c r="A11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="3">
+        <v>44304.8283912037</v>
+      </c>
+      <c r="F11" s="2">
+        <v>855994</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1922</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="2">
+        <v>25</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="3">
-        <v>44476.819409722222</v>
-      </c>
-      <c r="F12" s="2">
-        <v>481684</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1594</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="J12" s="2">
+      <c r="A12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="5">
+        <v>44266.709444444445</v>
+      </c>
+      <c r="F12" s="4">
+        <v>652159</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1235</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="4">
         <v>27</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>129</v>
+      <c r="K12" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E13" s="3">
-        <v>44528.770972222221</v>
+        <v>44476.819409722222</v>
       </c>
       <c r="F13" s="2">
-        <v>390914</v>
+        <v>481684</v>
       </c>
       <c r="G13" s="2">
-        <v>766</v>
+        <v>1594</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J13" s="2">
         <v>27</v>
@@ -1763,269 +1793,304 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E14" s="3">
-        <v>44425.667037037034</v>
+        <v>44528.770972222221</v>
       </c>
       <c r="F14" s="2">
-        <v>322022</v>
+        <v>390914</v>
       </c>
       <c r="G14" s="2">
-        <v>586</v>
+        <v>766</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J14" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="1">
-        <v>44487.583495370367</v>
-      </c>
-      <c r="F15">
-        <v>233330</v>
-      </c>
-      <c r="G15">
-        <v>1042</v>
-      </c>
-      <c r="H15" t="s">
-        <v>92</v>
-      </c>
-      <c r="I15" t="s">
-        <v>93</v>
-      </c>
-      <c r="J15">
-        <v>29</v>
+      <c r="A15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="3">
+        <v>44425.667037037034</v>
+      </c>
+      <c r="F15" s="2">
+        <v>322022</v>
+      </c>
+      <c r="G15" s="2">
+        <v>586</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="2">
+        <v>26</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="3">
-        <v>44420.645995370367</v>
-      </c>
-      <c r="F16" s="2">
-        <v>204551</v>
-      </c>
-      <c r="G16" s="2">
-        <v>954</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J16" s="2">
-        <v>27</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>129</v>
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="1">
+        <v>44487.583495370367</v>
+      </c>
+      <c r="F16">
+        <v>233330</v>
+      </c>
+      <c r="G16">
+        <v>1042</v>
+      </c>
+      <c r="H16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" s="1">
-        <v>44464.875011574077</v>
-      </c>
-      <c r="F17">
-        <v>191524</v>
-      </c>
-      <c r="G17">
-        <v>584</v>
-      </c>
-      <c r="H17" t="s">
-        <v>102</v>
-      </c>
-      <c r="I17" t="s">
-        <v>103</v>
-      </c>
-      <c r="J17">
-        <v>28</v>
+      <c r="A17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="3">
+        <v>44420.645995370367</v>
+      </c>
+      <c r="F17" s="2">
+        <v>204551</v>
+      </c>
+      <c r="G17" s="2">
+        <v>954</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" s="2">
+        <v>27</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E18" s="3">
-        <v>44368.520995370367</v>
-      </c>
-      <c r="F18" s="2">
-        <v>162805</v>
-      </c>
-      <c r="G18" s="2">
-        <v>511</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J18" s="2">
-        <v>27</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>129</v>
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" s="1">
+        <v>44464.875011574077</v>
+      </c>
+      <c r="F18">
+        <v>191524</v>
+      </c>
+      <c r="G18">
+        <v>584</v>
+      </c>
+      <c r="H18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" t="s">
+        <v>103</v>
+      </c>
+      <c r="J18">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" s="1">
-        <v>44503.58258101852</v>
-      </c>
-      <c r="F19">
-        <v>132500</v>
-      </c>
-      <c r="G19">
-        <v>786</v>
-      </c>
-      <c r="H19" t="s">
-        <v>114</v>
-      </c>
-      <c r="I19" t="s">
-        <v>115</v>
-      </c>
-      <c r="J19">
+      <c r="A19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="3">
+        <v>44368.520995370367</v>
+      </c>
+      <c r="F19" s="2">
+        <v>162805</v>
+      </c>
+      <c r="G19" s="2">
+        <v>511</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" s="2">
         <v>27</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E20" s="1">
-        <v>44373.583553240744</v>
+        <v>44503.58258101852</v>
       </c>
       <c r="F20">
-        <v>117855</v>
+        <v>132500</v>
       </c>
       <c r="G20">
-        <v>1078</v>
+        <v>786</v>
       </c>
       <c r="H20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="I20" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J20">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="1">
+        <v>44373.583553240744</v>
+      </c>
+      <c r="F21">
+        <v>117855</v>
+      </c>
+      <c r="G21">
+        <v>1078</v>
+      </c>
+      <c r="H21" t="s">
+        <v>120</v>
+      </c>
+      <c r="I21" t="s">
+        <v>121</v>
+      </c>
+      <c r="J21">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E22" s="3">
         <v>44399.770960648151</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F22" s="2">
         <v>106862</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G22" s="2">
         <v>507</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J22" s="2">
         <v>28</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>131</v>
       </c>
     </row>

</xml_diff>